<commit_message>
Elaboración del Diagrama del proceso de manufactura manual de las bicicletas
</commit_message>
<xml_diff>
--- a/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Tiempo estandar de manufacura manual.xlsx
+++ b/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Tiempo estandar de manufacura manual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\01 Investigación fabricación de bicicletas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\01 Investigación fabricación de bicicletas\03 Código y análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0454B47-852A-4B24-80E1-59A0016A9987}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569CD280-51C4-444E-89F3-E89A3CDEF6AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Numero
  de 
@@ -111,6 +111,51 @@
   </si>
   <si>
     <t>Rueda trasera y cadena - Colocación</t>
+  </si>
+  <si>
+    <t>Operario</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>D, E</t>
+  </si>
+  <si>
+    <t>F, G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -178,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +244,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,6 +541,7 @@
     <col min="3" max="3" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -508,7 +557,9 @@
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -530,8 +581,13 @@
         <f>_xlfn.CONCAT(QUOTIENT(D4,60),":",D4-(QUOTIENT(D4,60)*60))</f>
         <v>5:50,4</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="8">
+        <f>(D4/480)*100</f>
+        <v>73</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -552,8 +608,13 @@
         <f t="shared" ref="E5:E23" si="0">_xlfn.CONCAT(QUOTIENT(D5,60),":",D5-(QUOTIENT(D5,60)*60))</f>
         <v>6:24,8</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" ref="G5:G23" si="1">(D5/480)*100</f>
+        <v>80.166666666666657</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -574,8 +635,13 @@
         <f t="shared" si="0"/>
         <v>1:51,7</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="1"/>
+        <v>23.270833333333336</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -596,8 +662,13 @@
         <f t="shared" si="0"/>
         <v>12:24,8</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="8">
+        <f>((D7/480)*100)/2</f>
+        <v>77.583333333333329</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -618,8 +689,13 @@
         <f t="shared" si="0"/>
         <v>14:35,8</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="8">
+        <f>((D8/480)*100)/2</f>
+        <v>91.229166666666657</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -640,8 +716,13 @@
         <f t="shared" si="0"/>
         <v>0:22,8</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="F9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="1"/>
+        <v>4.75</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -662,8 +743,13 @@
         <f t="shared" si="0"/>
         <v>8:0</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -684,8 +770,13 @@
         <f t="shared" si="0"/>
         <v>7:42,1</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="1"/>
+        <v>96.270833333333343</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -706,8 +797,13 @@
         <f t="shared" si="0"/>
         <v>0:40,4</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="1"/>
+        <v>8.4166666666666661</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -728,8 +824,13 @@
         <f>_xlfn.CONCAT(QUOTIENT(D13,60),":",FIXED(D13-(QUOTIENT(D13,60)*60),1))</f>
         <v>3:2,8</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="1"/>
+        <v>38.083333333333336</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -750,8 +851,13 @@
         <f t="shared" si="0"/>
         <v>1:57,3</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="F14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="1"/>
+        <v>24.437499999999996</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -772,8 +878,13 @@
         <f t="shared" si="0"/>
         <v>1:29,2</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="1"/>
+        <v>18.583333333333336</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -794,8 +905,13 @@
         <f t="shared" si="0"/>
         <v>6:37,5</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="1"/>
+        <v>82.8125</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -816,8 +932,13 @@
         <f t="shared" si="0"/>
         <v>6:39,1</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="1"/>
+        <v>83.145833333333343</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -838,8 +959,13 @@
         <f t="shared" si="0"/>
         <v>5:35,2</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="1"/>
+        <v>69.833333333333343</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -860,8 +986,13 @@
         <f t="shared" si="0"/>
         <v>3:43,4</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="1"/>
+        <v>46.541666666666671</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -882,8 +1013,13 @@
         <f t="shared" si="0"/>
         <v>6:28,2</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="F20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="1"/>
+        <v>80.875</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -904,8 +1040,13 @@
         <f t="shared" si="0"/>
         <v>5:24,8</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="F21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="1"/>
+        <v>67.666666666666657</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -926,8 +1067,13 @@
         <f t="shared" si="0"/>
         <v>1:36,5</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="F22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" si="1"/>
+        <v>20.104166666666668</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -948,8 +1094,13 @@
         <f t="shared" si="0"/>
         <v>0:46,6</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="1"/>
+        <v>9.7083333333333339</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>

</xml_diff>

<commit_message>
Se avanza en la investigación y presentación de avance del proyecto
</commit_message>
<xml_diff>
--- a/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Tiempo estandar de manufacura manual.xlsx
+++ b/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Tiempo estandar de manufacura manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\01 Investigación fabricación de bicicletas\03 Código y análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569CD280-51C4-444E-89F3-E89A3CDEF6AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0C74FF-49CB-4375-9F21-981F4CC3B0D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={744AED2D-B55C-4D4E-9F5B-A8299128F2CF}</author>
+  </authors>
+  <commentList>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{744AED2D-B55C-4D4E-9F5B-A8299128F2CF}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Ojo es por soldadura no por marco. por marco se debe multiplicar por 12.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Numero
  de 
@@ -156,6 +174,20 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>Utilización 
+Operario [%]</t>
+  </si>
+  <si>
+    <t>Tiempo 
+por 
+pieza [s]</t>
+  </si>
+  <si>
+    <t>Cantidad
+de operaciones
+por turno</t>
   </si>
 </sst>
 </file>
@@ -165,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +212,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -246,7 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -264,6 +302,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Leonardo Fabio Mercado Benìtez" id="{CAF5515B-8733-4A0D-93D1-0648DD09DE2F}" userId="Leonardo Fabio Mercado Benìtez" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,12 +571,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F8" dT="2021-04-07T08:01:00.87" personId="{CAF5515B-8733-4A0D-93D1-0648DD09DE2F}" id="{744AED2D-B55C-4D4E-9F5B-A8299128F2CF}">
+    <text>Ojo es por soldadura no por marco. por marco se debe multiplicar por 12.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:L34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,11 +592,13 @@
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="3" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -554,20 +608,28 @@
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -577,24 +639,31 @@
       <c r="D4" s="2">
         <v>350.4</v>
       </c>
-      <c r="E4" s="2" t="str">
+      <c r="E4" s="2">
+        <v>1050</v>
+      </c>
+      <c r="F4" s="8">
+        <f>(D4/E4)*60</f>
+        <v>20.022857142857141</v>
+      </c>
+      <c r="G4" s="2" t="str">
         <f>_xlfn.CONCAT(QUOTIENT(D4,60),":",D4-(QUOTIENT(D4,60)*60))</f>
         <v>5:50,4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="8">
+      <c r="I4" s="8">
         <f>(D4/480)*100</f>
         <v>73</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -604,24 +673,31 @@
       <c r="D5" s="2">
         <v>384.8</v>
       </c>
-      <c r="E5" s="2" t="str">
-        <f t="shared" ref="E5:E23" si="0">_xlfn.CONCAT(QUOTIENT(D5,60),":",D5-(QUOTIENT(D5,60)*60))</f>
+      <c r="E5" s="2">
+        <v>648</v>
+      </c>
+      <c r="F5" s="8">
+        <f>(D5/E5)*60</f>
+        <v>35.629629629629633</v>
+      </c>
+      <c r="G5" s="2" t="str">
+        <f t="shared" ref="G5:G23" si="0">_xlfn.CONCAT(QUOTIENT(D5,60),":",D5-(QUOTIENT(D5,60)*60))</f>
         <v>6:24,8</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="8">
-        <f t="shared" ref="G5:G23" si="1">(D5/480)*100</f>
+      <c r="I5" s="8">
+        <f t="shared" ref="I5:I23" si="1">(D5/480)*100</f>
         <v>80.166666666666657</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -631,24 +707,31 @@
       <c r="D6" s="2">
         <v>111.7</v>
       </c>
-      <c r="E6" s="2" t="str">
+      <c r="E6" s="2">
+        <v>486</v>
+      </c>
+      <c r="F6" s="8">
+        <f>(D6/E6)*60</f>
+        <v>13.790123456790123</v>
+      </c>
+      <c r="G6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1:51,7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="8">
+      <c r="I6" s="8">
         <f t="shared" si="1"/>
         <v>23.270833333333336</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -658,24 +741,31 @@
       <c r="D7" s="2">
         <v>744.8</v>
       </c>
-      <c r="E7" s="2" t="str">
+      <c r="E7" s="2">
+        <v>1782</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" ref="F7:F23" si="2">(D7/E7)*60</f>
+        <v>25.077441077441076</v>
+      </c>
+      <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>12:24,8</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="8">
+      <c r="I7" s="8">
         <f>((D7/480)*100)/2</f>
         <v>77.583333333333329</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -685,24 +775,31 @@
       <c r="D8" s="7">
         <v>875.8</v>
       </c>
-      <c r="E8" s="2" t="str">
+      <c r="E8" s="7">
+        <v>972</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="2"/>
+        <v>54.061728395061728</v>
+      </c>
+      <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>14:35,8</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="8">
+      <c r="I8" s="8">
         <f>((D8/480)*100)/2</f>
         <v>91.229166666666657</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -712,24 +809,31 @@
       <c r="D9" s="2">
         <v>22.8</v>
       </c>
-      <c r="E9" s="2" t="str">
+      <c r="E9" s="2">
+        <v>81</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="2"/>
+        <v>16.888888888888889</v>
+      </c>
+      <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0:22,8</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="8">
+      <c r="I9" s="8">
         <f t="shared" si="1"/>
         <v>4.75</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
@@ -739,24 +843,29 @@
       <c r="D10" s="6">
         <v>480</v>
       </c>
-      <c r="E10" s="2" t="str">
+      <c r="E10" s="6"/>
+      <c r="F10" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>8:0</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="8">
+      <c r="I10" s="8">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -766,24 +875,29 @@
       <c r="D11" s="2">
         <v>462.1</v>
       </c>
-      <c r="E11" s="2" t="str">
+      <c r="E11" s="2"/>
+      <c r="F11" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>7:42,1</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="8">
+      <c r="I11" s="8">
         <f t="shared" si="1"/>
         <v>96.270833333333343</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -793,24 +907,29 @@
       <c r="D12" s="2">
         <v>40.4</v>
       </c>
-      <c r="E12" s="2" t="str">
+      <c r="E12" s="2"/>
+      <c r="F12" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0:40,4</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="8">
+      <c r="I12" s="8">
         <f t="shared" si="1"/>
         <v>8.4166666666666661</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>12</v>
       </c>
@@ -820,24 +939,29 @@
       <c r="D13" s="2">
         <v>182.8</v>
       </c>
-      <c r="E13" s="2" t="str">
+      <c r="E13" s="2"/>
+      <c r="F13" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="2" t="str">
         <f>_xlfn.CONCAT(QUOTIENT(D13,60),":",FIXED(D13-(QUOTIENT(D13,60)*60),1))</f>
         <v>3:2,8</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="8">
+      <c r="I13" s="8">
         <f t="shared" si="1"/>
         <v>38.083333333333336</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>13</v>
       </c>
@@ -847,24 +971,29 @@
       <c r="D14" s="2">
         <v>117.3</v>
       </c>
-      <c r="E14" s="2" t="str">
+      <c r="E14" s="2"/>
+      <c r="F14" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1:57,3</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="8">
+      <c r="I14" s="8">
         <f t="shared" si="1"/>
         <v>24.437499999999996</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <v>14</v>
       </c>
@@ -874,24 +1003,29 @@
       <c r="D15" s="2">
         <v>89.2</v>
       </c>
-      <c r="E15" s="2" t="str">
+      <c r="E15" s="2"/>
+      <c r="F15" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1:29,2</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="8">
+      <c r="I15" s="8">
         <f t="shared" si="1"/>
         <v>18.583333333333336</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>15</v>
       </c>
@@ -901,24 +1035,29 @@
       <c r="D16" s="2">
         <v>397.5</v>
       </c>
-      <c r="E16" s="2" t="str">
+      <c r="E16" s="2"/>
+      <c r="F16" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>6:37,5</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="8">
+      <c r="I16" s="8">
         <f t="shared" si="1"/>
         <v>82.8125</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>16</v>
       </c>
@@ -928,24 +1067,29 @@
       <c r="D17" s="2">
         <v>399.1</v>
       </c>
-      <c r="E17" s="2" t="str">
+      <c r="E17" s="2"/>
+      <c r="F17" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>6:39,1</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="8">
+      <c r="I17" s="8">
         <f t="shared" si="1"/>
         <v>83.145833333333343</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <v>17</v>
       </c>
@@ -955,24 +1099,29 @@
       <c r="D18" s="2">
         <v>335.2</v>
       </c>
-      <c r="E18" s="2" t="str">
+      <c r="E18" s="2"/>
+      <c r="F18" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>5:35,2</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="8">
+      <c r="I18" s="8">
         <f t="shared" si="1"/>
         <v>69.833333333333343</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>18</v>
       </c>
@@ -982,24 +1131,29 @@
       <c r="D19" s="2">
         <v>223.4</v>
       </c>
-      <c r="E19" s="2" t="str">
+      <c r="E19" s="2"/>
+      <c r="F19" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>3:43,4</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="8">
+      <c r="I19" s="8">
         <f t="shared" si="1"/>
         <v>46.541666666666671</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <v>19</v>
       </c>
@@ -1009,24 +1163,29 @@
       <c r="D20" s="2">
         <v>388.2</v>
       </c>
-      <c r="E20" s="2" t="str">
+      <c r="E20" s="2"/>
+      <c r="F20" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>6:28,2</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="8">
+      <c r="I20" s="8">
         <f t="shared" si="1"/>
         <v>80.875</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>20</v>
       </c>
@@ -1036,24 +1195,29 @@
       <c r="D21" s="2">
         <v>324.8</v>
       </c>
-      <c r="E21" s="2" t="str">
+      <c r="E21" s="2"/>
+      <c r="F21" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>5:24,8</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="8">
+      <c r="I21" s="8">
         <f t="shared" si="1"/>
         <v>67.666666666666657</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>21</v>
       </c>
@@ -1063,24 +1227,29 @@
       <c r="D22" s="2">
         <v>96.5</v>
       </c>
-      <c r="E22" s="2" t="str">
+      <c r="E22" s="2"/>
+      <c r="F22" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>1:36,5</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="8">
+      <c r="I22" s="8">
         <f t="shared" si="1"/>
         <v>20.104166666666668</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
         <v>22</v>
       </c>
@@ -1090,105 +1259,133 @@
       <c r="D23" s="2">
         <v>46.6</v>
       </c>
-      <c r="E23" s="2" t="str">
+      <c r="E23" s="2"/>
+      <c r="F23" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>0:46,6</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="8">
+      <c r="I23" s="8">
         <f t="shared" si="1"/>
         <v>9.7083333333333339</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit de urgencia para ordenar repositorio
</commit_message>
<xml_diff>
--- a/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Tiempo estandar de manufacura manual.xlsx
+++ b/01 Documentación/01 Investigación fabricación de bicicletas/03 Código y análisis/Tiempo estandar de manufacura manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\03 APM\04 Gitrespository\Proyecto_APM\01 Documentación\01 Investigación fabricación de bicicletas\03 Código y análisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0C74FF-49CB-4375-9F21-981F4CC3B0D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94186762-58C8-4131-AFA7-4EEFC619DB71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,12 +212,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -261,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,6 +279,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,10 +840,12 @@
       <c r="D10" s="6">
         <v>480</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="E10" s="9">
+        <v>243</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="2"/>
+        <v>118.5185185185185</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -875,10 +874,12 @@
       <c r="D11" s="2">
         <v>462.1</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="E11" s="2">
+        <v>243</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="2"/>
+        <v>114.09876543209877</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -907,10 +908,12 @@
       <c r="D12" s="2">
         <v>40.4</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="8" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="E12" s="2">
+        <v>162</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="2"/>
+        <v>14.962962962962962</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>